<commit_message>
Add report image file and other details
</commit_message>
<xml_diff>
--- a/automation/reports/mobiles.xlsx
+++ b/automation/reports/mobiles.xlsx
@@ -466,12 +466,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>iQOO Z10R 5G (Aquamarine, 8GB RAM, 256GB Storage) | 32MP 4K Selfie Camera | Quad-Curved AMOLED Display | Dimensity 7400 Processor with 750K+ AnTuTu</t>
+          <t>iQOO Z10 5G (Stellar Black, 12GB RAM, 256GB Storage) | India's Biggest Ever 7300 mAh Battery | Snapdragon 7s Gen 3 Processor | Brightest Quad Curved AMOLED Display in The Segment</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21,498</t>
+          <t>25,998</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -531,12 +531,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M06 5G (Sage Green, 6GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | 12 5G Bands| 25W Fast Charging | 4 Gen of OS Upgrades | Without Charger</t>
+          <t>realme NARZO 80 Pro 5G (Speed Silver,12GB+256GB) | Segment's 1st MediaTek Dimensity 7400 Chipset | 6000mAh Titan Battery + 80W Ultra Charge | 4500nits HyperGlow Esports Display | IP69 Waterproof</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>8,999</t>
+          <t>21,498</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -544,12 +544,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>realme NARZO 80 Pro 5G (Speed Silver,12GB+256GB) | Segment's 1st MediaTek Dimensity 7400 Chipset | 6000mAh Titan Battery + 80W Ultra Charge | 4500nits HyperGlow Esports Display | IP69 Waterproof</t>
+          <t>POCO C71, Desert Gold (6GB, 128GB)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>21,498</t>
+          <t>6,799</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -557,12 +557,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>POCO C71, Desert Gold (6GB, 128GB)</t>
+          <t>Redmi 15 5G Midnight Black 8GB + 256GB | Segment's Largest 7000mAhA Battery | Segment's Largest Display 17.53cm(6.9) Up to 144Hz | Snapdragon 6s Gen 3 | 18W Reverse Charging | 50MP AI Dual Camera</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6,799</t>
+          <t>16,998</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -570,12 +570,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Redmi 15 5G Midnight Black 8GB + 256GB | Segment's Largest 7000mAhA Battery | Segment's Largest Display 17.53cm(6.9) Up to 144Hz | Snapdragon 6s Gen 3 | 18W Reverse Charging | 50MP AI Dual Camera</t>
+          <t>Samsung Galaxy M06 5G (Sage Green, 6GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | 12 5G Bands| 25W Fast Charging | 4 Gen of OS Upgrades | Without Charger</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16,998</t>
+          <t>8,999</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -583,12 +583,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>iQOO Z10 5G (Glacier Silver, 12GB RAM, 256GB Storage) | India's Biggest Ever 7300 mAh Battery | Snapdragon 7s Gen 3 Processor | Brightest Quad Curved AMOLED Display in The Segment</t>
+          <t>Samsung Galaxy A55 5G (Awesome Iceblue, 8GB RAM, 128GB Storage) | AI | Metal Frame | 50 MP Main Camera (OIS) | Super HDR Video| Nightography | IP67 | Corning Gorilla Glass Victus+ | sAMOLED Display</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>25,998</t>
+          <t>23,999</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -700,12 +700,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>OnePlus Nord 5 | Snapdragon 8s Gen 3 | Stable 144FPS Gaming | Dual 50MP Flagship Camera | Powered by OnePlus AI | 12GB + 256GB | Dry Ice</t>
+          <t>Nokia All-New 105 Single Sim Keypad Phone with Built-in UPI Payments, Long-Lasting Battery, Wireless FM Radio | Red</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>34,998</t>
+          <t>1,199</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>

</xml_diff>

<commit_message>
Refactor API tests for user creation, update, and deletion; enhance logging and assertions
- Removed redundant test for user login and consolidated user creation logic.
- Updated assertions to check for specific response fields.
- Improved logging for better traceability during test execution.
- Simplified WebDriver setup in UI tests, focusing on Chrome.
- Adjusted test assertions to ensure at least one result is returned.
- Centralized file path management in common_methods for better maintainability.
- Enhanced ConfigManager to dynamically locate the configuration file.
- Added pytest configuration for better test reporting and logging.
- Created requirements.txt to manage project dependencies.
</commit_message>
<xml_diff>
--- a/automation/reports/mobiles.xlsx
+++ b/automation/reports/mobiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,45 +436,68 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>Price</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>rating</t>
+          <t>Rating</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Reviews</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samsung Galaxy S24 Ultra 5G AI Smartphone with Galaxy AI (Titanium Gray, 12GB, 256GB Storage), Snapdragon 8 Gen 3, 200 MP Camera with ProVisual Engine and 5000mAh Battery</t>
+          <t>iPhone Air 256 GB: Thinnest iPhone Ever, 16.63 cm (6.5″) Display with Promotion up to 120Hz, Powerful A19 Pro Chip, Center Stage Front Camera, All-Day Battery Life; Light Gold</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>97,999</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>1,19,900</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>5,050</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>iQOO Z10 5G (Stellar Black, 12GB RAM, 256GB Storage) | India's Biggest Ever 7300 mAh Battery | Snapdragon 7s Gen 3 Processor | Brightest Quad Curved AMOLED Display in The Segment</t>
+          <t>Apple iPhone 15 (128 GB) - Blue</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>25,998</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>47,999</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>6,910</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -487,228 +510,390 @@
           <t>6,249</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2,160</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>OnePlus Nord CE4 Lite 5G (Super Silver, 8GB RAM, 128GB Storage) | Lifetime Display Warranty | 5500 mAh Battery, 80W SUPERVOOC and Reverse Charging | 50MP Camera with OIS | 120Hz AMOLED Display</t>
+          <t>iQOO Z10 Lite 5G (Cyber Green, 6GB RAM, 128GB Storage) | 6000 mAh Battery | Dimensity 6300 5G Processor with 433K+* AnTuTu Score | IP64 Rated &amp; Military Grade Shock-Resistance*</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16,998</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
+          <t>10,998</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>iQOO Z10 Lite 5G (Cyber Green, 6GB RAM, 128GB Storage) | 6000 mAh Battery | Dimensity 6300 5G Processor with 433K+* AnTuTu Score | IP64 Rated &amp; Military Grade Shock-Resistance*</t>
+          <t>Pova Slim 5G (Slim White, 8+128GB) | World's Slimmest and Lightest* 5G with 5160mAh Battery | World's 1st Dynamic Mood Light | 144Hz 1.5K 3D Curve AMOLED | Military Grade MIL 810H Protection | IP64</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10,998</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>19,999</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2,939</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>POCO C71, Cool Blue (6GB, 128GB)</t>
+          <t>Samsung Galaxy M06 5G (Sage Green, 6GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | 12 5G Bands| 25W Fast Charging | 4 Gen of OS Upgrades | Without Charger</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6,989</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
+          <t>8,999</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2,271</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>realme NARZO 80 Pro 5G (Speed Silver,12GB+256GB) | Segment's 1st MediaTek Dimensity 7400 Chipset | 6000mAh Titan Battery + 80W Ultra Charge | 4500nits HyperGlow Esports Display | IP69 Waterproof</t>
+          <t>Samsung Galaxy M16 5G (Thunder Black, 6GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | Super Amoled Display | AI | 25W Fast Charging | 6 Gen of OS Upgrades | Without Charger</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21,498</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
+          <t>11,749</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>556</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>POCO C71, Desert Gold (6GB, 128GB)</t>
+          <t>POCO C71, Cool Blue (6GB, 128GB)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6,799</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>6,798</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>9,493</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Redmi 15 5G Midnight Black 8GB + 256GB | Segment's Largest 7000mAhA Battery | Segment's Largest Display 17.53cm(6.9) Up to 144Hz | Snapdragon 6s Gen 3 | 18W Reverse Charging | 50MP AI Dual Camera</t>
+          <t>realme 14X 5G Smartphone Dimensity 6300 6nm Chip 8GB RAM 128GB ROM 6.67 Inch HD+ IP69 Waterproof 6000mAh Battery 45W Fast Charge Support Fingerprint GPS WiFi Bluetooth (Gold)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16,998</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>14,190</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1,464</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M06 5G (Sage Green, 6GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | 12 5G Bands| 25W Fast Charging | 4 Gen of OS Upgrades | Without Charger</t>
+          <t>OnePlus Nord CE4 Lite 5G (Super Silver, 8GB RAM, 128GB Storage) | Lifetime Display Warranty | 5500 mAh Battery, 80W SUPERVOOC and Reverse Charging | 50MP Camera with OIS | 120Hz AMOLED Display</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>8,999</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>16,998</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1,794</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A55 5G (Awesome Iceblue, 8GB RAM, 128GB Storage) | AI | Metal Frame | 50 MP Main Camera (OIS) | Super HDR Video| Nightography | IP67 | Corning Gorilla Glass Victus+ | sAMOLED Display</t>
+          <t>iPhone 16 128 GB: 5G Mobile Phone with Camera Control, A18 Chip and a Big Boost in Battery Life. Works with AirPods; White</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>23,999</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+          <t>69,499</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2,016</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lava Bold N1 Pro (Stealth Black, 4 GB RAM, 128 GB Storage)| Bigger 6.67" HD+ IP54 Display | 120 Hz Refresh Rate | 50 MP AI Triple Rear Camera | 8 MP Front Camera| 5000 mAh Battery| Charger in Box</t>
+          <t>Apple iPhone 15 Plus (128 GB) - Black</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>6,849</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>68,999</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2,271</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M35 5G (DayBreak Blue,8GB RAM,128GB Storage)| Corning Gorilla Glass Victus+| AnTuTu Score 595K+| Vapour Cooling Chamber| 6000mAh Battery| 120Hz Super AMOLED Display| AI| Without Charger</t>
+          <t>Redmi 13 5G Prime Edition, Orchid Pink, 8GB+128GB | India Debut SD 4 Gen 2 AE | 108MP Pro Grade Camera | 6.79in Largest Display in Segment</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>18,499</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
+          <t>11,199</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1,138</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>iQOO Z10 Lite 5G (Cyber Green, 4GB RAM, 128GB Storage) | 6000 mAh Battery | Dimensity 6300 5G Processor with 433K+* AnTuTu Score | IP64 Rated &amp; Military Grade Shock-Resistance*</t>
+          <t>Samsung Galaxy M16 5G (Blush Pink, 4GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | Super Amoled Display | AI | 25W Fast Charging | 6 Gen of OS Upgrades | Without Charger</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>9,998</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
+          <t>10,499</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>556</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M16 5G (Blush Pink, 4GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | Super Amoled Display | AI | 25W Fast Charging | 6 Gen of OS Upgrades | Without Charger</t>
+          <t>realme NARZO 80 Pro 5G (Speed Silver,12GB+256GB) | Segment's 1st MediaTek Dimensity 7400 Chipset | 6000mAh Titan Battery + 80W Ultra Charge | 4500nits HyperGlow Esports Display | IP69 Waterproof</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10,749</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
+          <t>21,498</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>realme NARZO 80 Lite 5G (Crystal Purple, 6GB+128GB) | 6000mAh Long-Lasting Battery | MediaTek Dimensity 6300 5G | AI Assist | IP64 Rated Water &amp; Dust Resistance | Military-Grade Durability</t>
+          <t>POCO C71, Desert Gold (6GB, 128GB)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10,998</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+          <t>6,799</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>19,655</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>POCO M6 Plus 5G Misty Lavender 8GB RAM 128GB ROM</t>
+          <t>Redmi 15 5G Midnight Black 8GB + 256GB | Segment's Largest 7000mAhA Battery | Segment's Largest Display 17.53cm(6.9) Up to 144Hz | Snapdragon 6s Gen 3 | 18W Reverse Charging | 50MP AI Dual Camera</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10,299</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
+          <t>16,998</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2,016</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M06 5G (Sage Green, 4GB RAM, 64GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | 12 5G Bands| 25W Fast Charging | 4 Gen of OS Upgrades | Without Charger</t>
+          <t>Nokia 105 Classic | Single SIM Keypad Phone with Built-in UPI Payments, Long-Lasting Battery, Wireless FM Radio, Without Charger | Charcoal</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7,499</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
+          <t>949</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2,939</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M16 5G (Thunder Black, 6GB RAM, 128 GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | Super Amoled Display | AI | 25W Fast Charging | 6 Gen of OS Upgrades | Without Charger</t>
+          <t>Redmi 13 5G Prime Edition, Black Diamond, 8GB+128GB | India Debut SD 4 Gen 2 AE | 108MP Pro Grade Camera | 6.79in Largest Display in Segment</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11,999</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
+          <t>11,199</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2,446</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Nokia All-New 105 Single Sim Keypad Phone with Built-in UPI Payments, Long-Lasting Battery, Wireless FM Radio | Red</t>
+          <t>Samsung Galaxy M06 5G (Sage Green, 4GB RAM, 64GB Storage) | MediaTek Dimensity 6300 | AnTuTu Score 422K+ | 12 5G Bands| 25W Fast Charging | 4 Gen of OS Upgrades | Without Charger</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1,199</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
+          <t>7,499</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>